<commit_message>
Update 006/008 conversion (#175)
Add media property to instance from "form of item" value (BOOKS/23).
</commit_message>
<xml_diff>
--- a/spec/ConvSpec-006-008-v1.6.xlsx
+++ b/spec/ConvSpec-006-008-v1.6.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1470" uniqueCount="1192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1479" uniqueCount="1196">
   <si>
     <t>ignore</t>
   </si>
@@ -3194,9 +3194,6 @@
     <t>006 - FIXED-LENGTH DATA ELEMENTS-- ADDITIONAL MATERIAL CHARACTERISTICS (R)</t>
   </si>
   <si>
-    <t>Add rdfs:label "large print"</t>
-  </si>
-  <si>
     <t>I - fontSize - FontSize - http://id.loc.gov/vocabulary/mfont/lp</t>
   </si>
   <si>
@@ -3425,9 +3422,6 @@
     <t>Add rdfs:label "phonodisc"</t>
   </si>
   <si>
-    <t>Add rdfs:label "braille code"</t>
-  </si>
-  <si>
     <t>Add rdfs:label "festschriften"</t>
   </si>
   <si>
@@ -3646,10 +3640,28 @@
     <t>add noteType "form of original item"</t>
   </si>
   <si>
-    <t>Fields 006, 008 - Fixed general and additional - v1.6, 07/08/2020</t>
-  </si>
-  <si>
     <t>I - issuance - Issuance - http://id.loc.gov/vocabulary/issuance/serl (if not already generated by LDR/07)</t>
+  </si>
+  <si>
+    <t>Add rdfs:label "large print" ; If MARC tag 338 $a does not exist, then I - carrier - Carrier - http://id.loc.gov/vocabulary/carriers/nc ; add rdfs:label "volume"</t>
+  </si>
+  <si>
+    <t>Add rdfs:label "braille code" ; If MARC tag 338 $a does not exist, then I - carrier - Carrier - http://id.loc.gov/vocabulary/carriers/nc ; add rdfs:label "volume"</t>
+  </si>
+  <si>
+    <t>Conversion 3</t>
+  </si>
+  <si>
+    <t>If MARC tag 337 $a does not exist, then I - media -Media - http://id.loc.gov/vocabulary/mediaTypes/n ; add rdfs:label "unmediated"</t>
+  </si>
+  <si>
+    <t>Fields 006, 008 - Fixed general and additional - v1.6, 08/17/2020</t>
+  </si>
+  <si>
+    <t>If MARC tag 337 $a does not exist, then I - media - Media - http://id.loc.gov/vocabulary/mediaTypes/n ; add rdfs:label "unmediated"</t>
+  </si>
+  <si>
+    <t>If MARC tag 337 $a does not exist, then I - media - Media - http://id.loc.gov/vocabulary/mediaTypes/c ; add rdfs:label "computer"</t>
   </si>
 </sst>
 </file>
@@ -3699,7 +3711,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3709,6 +3721,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3741,7 +3759,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -3774,6 +3792,15 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4059,8 +4086,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F581"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A279" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A280" sqref="A280:C290"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D108" sqref="D108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -4068,16 +4095,16 @@
     <col min="1" max="1" width="34.58203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="42.08203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="23.83203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11" style="1" customWidth="1"/>
-    <col min="5" max="5" width="31.75" style="1" customWidth="1"/>
+    <col min="4" max="4" width="31.75" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11" style="1" customWidth="1"/>
     <col min="6" max="6" width="19.75" style="1" customWidth="1"/>
     <col min="7" max="7" width="13.58203125" style="1" customWidth="1"/>
     <col min="8" max="16384" width="10.58203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="3" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" s="3" customFormat="1" ht="31" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>1190</v>
+        <v>1193</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>492</v>
@@ -4086,10 +4113,13 @@
         <v>493</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>1191</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>540</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="3" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" s="3" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>1045</v>
       </c>
@@ -4097,7 +4127,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>542</v>
       </c>
@@ -4105,7 +4135,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>557</v>
       </c>
@@ -4113,7 +4143,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>543</v>
       </c>
@@ -4121,7 +4151,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="4" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" s="4" customFormat="1" ht="31" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>544</v>
       </c>
@@ -4129,7 +4159,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>545</v>
       </c>
@@ -4137,7 +4167,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>546</v>
       </c>
@@ -4145,7 +4175,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>547</v>
       </c>
@@ -4153,7 +4183,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>548</v>
       </c>
@@ -4161,7 +4191,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="11" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>556</v>
       </c>
@@ -4169,7 +4199,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="12" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>549</v>
       </c>
@@ -4177,7 +4207,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="13" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>550</v>
       </c>
@@ -4185,7 +4215,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="14" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>555</v>
       </c>
@@ -4193,7 +4223,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="15" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
         <v>551</v>
       </c>
@@ -4201,7 +4231,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="16" spans="1:4" s="4" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" s="4" customFormat="1" ht="31" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
         <v>552</v>
       </c>
@@ -4209,7 +4239,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="17" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
         <v>553</v>
       </c>
@@ -4217,7 +4247,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="18" spans="1:5" s="4" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" s="4" customFormat="1" ht="31" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
         <v>554</v>
       </c>
@@ -4225,17 +4255,17 @@
         <v>562</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" ht="31" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="62" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" ht="62" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>46</v>
       </c>
@@ -4243,7 +4273,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>47</v>
       </c>
@@ -4251,7 +4281,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" ht="31" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>48</v>
       </c>
@@ -4259,24 +4289,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="62" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" ht="62" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>1187</v>
-      </c>
-      <c r="E25" s="9"/>
-    </row>
-    <row r="26" spans="1:5" ht="62" x14ac:dyDescent="0.35">
+        <v>1185</v>
+      </c>
+      <c r="D25" s="9"/>
+    </row>
+    <row r="26" spans="1:4" ht="62" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>1188</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="77.5" x14ac:dyDescent="0.35">
+        <v>1186</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>51</v>
       </c>
@@ -4284,31 +4314,31 @@
         <v>613</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="62" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" ht="62" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>1092</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="62" x14ac:dyDescent="0.35">
+        <v>1091</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="62" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>1093</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
+        <v>1092</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>54</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>1094</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+        <v>1093</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>55</v>
       </c>
@@ -4316,24 +4346,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="93" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" ht="93" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>56</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>614</v>
       </c>
-      <c r="E32" s="9"/>
+      <c r="D32" s="9"/>
     </row>
     <row r="33" spans="1:5" ht="62" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
@@ -4341,7 +4371,7 @@
         <v>58</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>566</v>
@@ -4352,7 +4382,7 @@
         <v>59</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="62" x14ac:dyDescent="0.35">
@@ -4360,10 +4390,10 @@
         <v>60</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>1154</v>
+        <v>1152</v>
       </c>
       <c r="D36" s="9"/>
       <c r="E36" s="9"/>
@@ -4373,7 +4403,7 @@
         <v>61</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="C37" s="9"/>
     </row>
@@ -4441,16 +4471,16 @@
         <v>25</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>67</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>1090</v>
-      </c>
-      <c r="E49" s="9"/>
-    </row>
-    <row r="50" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
+        <v>1089</v>
+      </c>
+      <c r="D49" s="9"/>
+    </row>
+    <row r="50" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
         <v>68</v>
       </c>
@@ -4458,7 +4488,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
         <v>69</v>
       </c>
@@ -4466,42 +4496,42 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:4" ht="31" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:4" ht="31" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
         <v>76</v>
       </c>
@@ -4509,27 +4539,27 @@
         <v>514</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
         <v>25</v>
       </c>
@@ -4695,7 +4725,7 @@
         <v>580</v>
       </c>
       <c r="C82" s="5" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="31" x14ac:dyDescent="0.35">
@@ -4845,14 +4875,20 @@
         <v>108</v>
       </c>
       <c r="B97" s="9"/>
-      <c r="E97" s="9"/>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A98" s="1" t="s">
+      <c r="D97" s="9"/>
+    </row>
+    <row r="98" spans="1:6" s="12" customFormat="1" ht="93" x14ac:dyDescent="0.35">
+      <c r="A98" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="B98" s="1" t="s">
-        <v>0</v>
+      <c r="B98" s="13" t="s">
+        <v>1107</v>
+      </c>
+      <c r="C98" s="13" t="s">
+        <v>1112</v>
+      </c>
+      <c r="D98" s="13" t="s">
+        <v>1194</v>
       </c>
     </row>
     <row r="99" spans="1:6" ht="93" x14ac:dyDescent="0.35">
@@ -4860,15 +4896,15 @@
         <v>110</v>
       </c>
       <c r="B99" s="5" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="C99" s="5" t="s">
-        <v>1145</v>
-      </c>
-      <c r="D99" s="1" t="s">
-        <v>1058</v>
-      </c>
-      <c r="E99" s="9"/>
+        <v>1143</v>
+      </c>
+      <c r="D99" s="9"/>
+      <c r="E99" s="1" t="s">
+        <v>1057</v>
+      </c>
       <c r="F99" s="9"/>
     </row>
     <row r="100" spans="1:6" ht="93" x14ac:dyDescent="0.35">
@@ -4876,13 +4912,13 @@
         <v>111</v>
       </c>
       <c r="B100" s="5" t="s">
+        <v>1107</v>
+      </c>
+      <c r="C100" s="5" t="s">
         <v>1108</v>
       </c>
-      <c r="C100" s="5" t="s">
-        <v>1109</v>
-      </c>
-      <c r="D100" s="1" t="s">
-        <v>1057</v>
+      <c r="E100" s="1" t="s">
+        <v>1056</v>
       </c>
     </row>
     <row r="101" spans="1:6" ht="93" x14ac:dyDescent="0.35">
@@ -4890,101 +4926,116 @@
         <v>112</v>
       </c>
       <c r="B101" s="5" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="C101" s="5" t="s">
+        <v>1109</v>
+      </c>
+      <c r="E101" s="1" t="s">
+        <v>1055</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" s="12" customFormat="1" ht="108.5" x14ac:dyDescent="0.35">
+      <c r="A102" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="B102" s="14" t="s">
+        <v>1046</v>
+      </c>
+      <c r="C102" s="13" t="s">
+        <v>1189</v>
+      </c>
+      <c r="D102" s="13" t="s">
+        <v>1192</v>
+      </c>
+      <c r="E102" s="12" t="s">
+        <v>1054</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" s="12" customFormat="1" ht="108.5" x14ac:dyDescent="0.35">
+      <c r="A103" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="B103" s="14" t="s">
+        <v>999</v>
+      </c>
+      <c r="C103" s="13" t="s">
+        <v>1190</v>
+      </c>
+      <c r="D103" s="13" t="s">
+        <v>1192</v>
+      </c>
+      <c r="E103" s="12" t="s">
+        <v>1053</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" s="12" customFormat="1" ht="93" x14ac:dyDescent="0.35">
+      <c r="A104" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="B104" s="13" t="s">
+        <v>1107</v>
+      </c>
+      <c r="C104" s="13" t="s">
         <v>1110</v>
       </c>
-      <c r="D101" s="1" t="s">
-        <v>1056</v>
-      </c>
-    </row>
-    <row r="102" spans="1:6" ht="31" x14ac:dyDescent="0.35">
-      <c r="A102" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="B102" s="6" t="s">
-        <v>1047</v>
-      </c>
-      <c r="C102" s="6" t="s">
-        <v>1046</v>
-      </c>
-      <c r="D102" s="1" t="s">
-        <v>1055</v>
-      </c>
-    </row>
-    <row r="103" spans="1:6" ht="31" x14ac:dyDescent="0.35">
-      <c r="A103" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="B103" s="6" t="s">
-        <v>999</v>
-      </c>
-      <c r="C103" s="5" t="s">
-        <v>1117</v>
-      </c>
-      <c r="D103" s="1" t="s">
-        <v>1054</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6" ht="93" x14ac:dyDescent="0.35">
-      <c r="A104" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="B104" s="5" t="s">
-        <v>1108</v>
-      </c>
-      <c r="C104" s="5" t="s">
+      <c r="D104" s="13" t="s">
+        <v>1195</v>
+      </c>
+      <c r="E104" s="12" t="s">
+        <v>1052</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" s="12" customFormat="1" ht="108.5" x14ac:dyDescent="0.35">
+      <c r="A105" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="B105" s="13" t="s">
+        <v>1107</v>
+      </c>
+      <c r="C105" s="13" t="s">
         <v>1111</v>
       </c>
-      <c r="D104" s="1" t="s">
-        <v>1053</v>
-      </c>
-    </row>
-    <row r="105" spans="1:6" ht="108.5" x14ac:dyDescent="0.35">
-      <c r="A105" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="B105" s="5" t="s">
-        <v>1108</v>
-      </c>
-      <c r="C105" s="5" t="s">
+      <c r="D105" s="13" t="s">
+        <v>1195</v>
+      </c>
+      <c r="E105" s="12" t="s">
+        <v>1051</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" s="12" customFormat="1" ht="93" x14ac:dyDescent="0.35">
+      <c r="A106" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="B106" s="13" t="s">
+        <v>1107</v>
+      </c>
+      <c r="C106" s="13" t="s">
         <v>1112</v>
       </c>
-      <c r="D105" s="1" t="s">
-        <v>1052</v>
-      </c>
-      <c r="E105" s="6"/>
-    </row>
-    <row r="106" spans="1:6" ht="93" x14ac:dyDescent="0.35">
-      <c r="A106" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="B106" s="5" t="s">
-        <v>1108</v>
-      </c>
-      <c r="C106" s="5" t="s">
-        <v>1113</v>
-      </c>
-      <c r="D106" s="1" t="s">
-        <v>1051</v>
-      </c>
-      <c r="E106" s="6"/>
-    </row>
-    <row r="107" spans="1:6" ht="108.5" x14ac:dyDescent="0.35">
-      <c r="A107" s="1" t="s">
+      <c r="D106" s="13" t="s">
+        <v>1194</v>
+      </c>
+      <c r="E106" s="12" t="s">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" s="12" customFormat="1" ht="108.5" x14ac:dyDescent="0.35">
+      <c r="A107" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="B107" s="5" t="s">
-        <v>1108</v>
-      </c>
-      <c r="C107" s="5" t="s">
-        <v>1112</v>
-      </c>
-      <c r="D107" s="1" t="s">
-        <v>1050</v>
-      </c>
-      <c r="E107" s="6"/>
+      <c r="B107" s="13" t="s">
+        <v>1107</v>
+      </c>
+      <c r="C107" s="13" t="s">
+        <v>1111</v>
+      </c>
+      <c r="D107" s="13" t="s">
+        <v>1195</v>
+      </c>
+      <c r="E107" s="12" t="s">
+        <v>1049</v>
+      </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A108" s="1" t="s">
@@ -4999,9 +5050,9 @@
         <v>119</v>
       </c>
       <c r="B109" s="11" t="s">
-        <v>1103</v>
-      </c>
-      <c r="E109" s="9"/>
+        <v>1102</v>
+      </c>
+      <c r="D109" s="9"/>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A110" s="1" t="s">
@@ -5025,7 +5076,7 @@
         <v>122</v>
       </c>
       <c r="B112" s="5" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="C112" s="5" t="s">
         <v>1002</v>
@@ -5100,10 +5151,10 @@
         <v>128</v>
       </c>
       <c r="B119" s="5" t="s">
+        <v>1113</v>
+      </c>
+      <c r="C119" s="5" t="s">
         <v>1114</v>
-      </c>
-      <c r="C119" s="5" t="s">
-        <v>1115</v>
       </c>
     </row>
     <row r="120" spans="1:6" ht="46.5" x14ac:dyDescent="0.35">
@@ -5122,7 +5173,7 @@
         <v>130</v>
       </c>
       <c r="B121" s="5" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="C121" s="5" t="s">
         <v>1001</v>
@@ -5158,7 +5209,7 @@
         <v>514</v>
       </c>
       <c r="F124" s="1" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.35">
@@ -5184,7 +5235,7 @@
         <v>136</v>
       </c>
       <c r="B127" s="5" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="C127" s="1" t="s">
         <v>4</v>
@@ -5232,7 +5283,7 @@
       </c>
       <c r="C131" s="6"/>
       <c r="F131" s="1" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="132" spans="1:6" ht="46.5" x14ac:dyDescent="0.35">
@@ -5287,7 +5338,7 @@
         <v>514</v>
       </c>
       <c r="F136" s="1" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="137" spans="1:6" ht="46.5" x14ac:dyDescent="0.35">
@@ -5306,10 +5357,10 @@
         <v>147</v>
       </c>
       <c r="B138" s="5" t="s">
+        <v>1105</v>
+      </c>
+      <c r="C138" s="5" t="s">
         <v>1106</v>
-      </c>
-      <c r="C138" s="5" t="s">
-        <v>1107</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.35">
@@ -5325,7 +5376,7 @@
         <v>148</v>
       </c>
       <c r="B140" s="11" t="s">
-        <v>1157</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.35">
@@ -5341,13 +5392,13 @@
         <v>150</v>
       </c>
       <c r="B142" s="11" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="C142" s="5" t="s">
-        <v>1158</v>
-      </c>
-      <c r="E142" s="1" t="s">
-        <v>1146</v>
+        <v>1156</v>
+      </c>
+      <c r="D142" s="1" t="s">
+        <v>1144</v>
       </c>
     </row>
     <row r="143" spans="1:6" ht="31" x14ac:dyDescent="0.35">
@@ -5355,13 +5406,13 @@
         <v>151</v>
       </c>
       <c r="B143" s="11" t="s">
-        <v>1160</v>
+        <v>1158</v>
       </c>
       <c r="C143" s="5" t="s">
-        <v>1161</v>
-      </c>
-      <c r="E143" s="1" t="s">
-        <v>1147</v>
+        <v>1159</v>
+      </c>
+      <c r="D143" s="1" t="s">
+        <v>1145</v>
       </c>
     </row>
     <row r="144" spans="1:6" ht="31" x14ac:dyDescent="0.35">
@@ -5369,86 +5420,86 @@
         <v>152</v>
       </c>
       <c r="B144" s="11" t="s">
-        <v>1162</v>
+        <v>1160</v>
       </c>
       <c r="C144" s="5" t="s">
-        <v>1163</v>
-      </c>
-      <c r="E144" s="1" t="s">
-        <v>1148</v>
-      </c>
-    </row>
-    <row r="145" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
+        <v>1161</v>
+      </c>
+      <c r="D144" s="1" t="s">
+        <v>1146</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A145" s="1" t="s">
         <v>153</v>
       </c>
       <c r="B145" s="11" t="s">
-        <v>1164</v>
+        <v>1162</v>
       </c>
       <c r="C145" s="5" t="s">
-        <v>1165</v>
-      </c>
-      <c r="E145" s="1" t="s">
-        <v>1149</v>
-      </c>
-    </row>
-    <row r="146" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+        <v>1163</v>
+      </c>
+      <c r="D145" s="1" t="s">
+        <v>1147</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" ht="31" x14ac:dyDescent="0.35">
       <c r="A146" s="1" t="s">
         <v>154</v>
       </c>
       <c r="B146" s="11" t="s">
-        <v>1166</v>
+        <v>1164</v>
       </c>
       <c r="C146" s="5" t="s">
-        <v>1167</v>
-      </c>
-      <c r="E146" s="1" t="s">
-        <v>1150</v>
-      </c>
-    </row>
-    <row r="147" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+        <v>1165</v>
+      </c>
+      <c r="D146" s="1" t="s">
+        <v>1148</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" ht="31" x14ac:dyDescent="0.35">
       <c r="A147" s="1" t="s">
         <v>155</v>
       </c>
       <c r="B147" s="11" t="s">
-        <v>1168</v>
+        <v>1166</v>
       </c>
       <c r="C147" s="5" t="s">
-        <v>1169</v>
-      </c>
-      <c r="E147" s="1" t="s">
-        <v>1151</v>
-      </c>
-    </row>
-    <row r="148" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+        <v>1167</v>
+      </c>
+      <c r="D147" s="1" t="s">
+        <v>1149</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" ht="31" x14ac:dyDescent="0.35">
       <c r="A148" s="1" t="s">
         <v>156</v>
       </c>
       <c r="B148" s="11" t="s">
-        <v>1170</v>
+        <v>1168</v>
       </c>
       <c r="C148" s="5" t="s">
-        <v>1171</v>
-      </c>
-      <c r="E148" s="1" t="s">
-        <v>1152</v>
-      </c>
-    </row>
-    <row r="149" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+        <v>1169</v>
+      </c>
+      <c r="D148" s="1" t="s">
+        <v>1150</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" ht="31" x14ac:dyDescent="0.35">
       <c r="A149" s="1" t="s">
         <v>157</v>
       </c>
       <c r="B149" s="11" t="s">
-        <v>1172</v>
+        <v>1170</v>
       </c>
       <c r="C149" s="5" t="s">
-        <v>1173</v>
-      </c>
-      <c r="E149" s="1" t="s">
-        <v>1153</v>
-      </c>
-    </row>
-    <row r="150" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+        <v>1171</v>
+      </c>
+      <c r="D149" s="1" t="s">
+        <v>1151</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" ht="31" x14ac:dyDescent="0.35">
       <c r="A150" s="1" t="s">
         <v>158</v>
       </c>
@@ -5456,7 +5507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A151" s="1" t="s">
         <v>24</v>
       </c>
@@ -5464,7 +5515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A152" s="1" t="s">
         <v>25</v>
       </c>
@@ -5472,7 +5523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A153" s="1" t="s">
         <v>159</v>
       </c>
@@ -5480,7 +5531,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A154" s="1" t="s">
         <v>160</v>
       </c>
@@ -5488,7 +5539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A155" s="1" t="s">
         <v>161</v>
       </c>
@@ -5499,7 +5550,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A156" s="1" t="s">
         <v>25</v>
       </c>
@@ -5507,7 +5558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A157" s="1" t="s">
         <v>162</v>
       </c>
@@ -5515,7 +5566,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A158" s="1" t="s">
         <v>163</v>
       </c>
@@ -5523,7 +5574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A159" s="1" t="s">
         <v>164</v>
       </c>
@@ -5531,10 +5582,10 @@
         <v>644</v>
       </c>
       <c r="C159" s="5" t="s">
-        <v>1118</v>
-      </c>
-    </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.35">
+        <v>1116</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A160" s="1" t="s">
         <v>25</v>
       </c>
@@ -5560,10 +5611,10 @@
         <v>167</v>
       </c>
       <c r="B163" s="10" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="C163" s="5" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.35">
@@ -5823,10 +5874,10 @@
         <v>115</v>
       </c>
       <c r="B192" s="5" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="C192" s="5" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="193" spans="1:3" ht="108.5" x14ac:dyDescent="0.35">
@@ -5834,10 +5885,10 @@
         <v>116</v>
       </c>
       <c r="B193" s="5" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="C193" s="5" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.35">
@@ -6733,10 +6784,10 @@
         <v>268</v>
       </c>
       <c r="B282" s="11" t="s">
-        <v>1191</v>
+        <v>1188</v>
       </c>
       <c r="C282" s="11" t="s">
-        <v>1155</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.35">
@@ -6891,7 +6942,7 @@
         <v>837</v>
       </c>
       <c r="C300" s="5" t="s">
-        <v>1119</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="301" spans="1:3" ht="46.5" x14ac:dyDescent="0.35">
@@ -7031,7 +7082,7 @@
         <v>678</v>
       </c>
       <c r="C315" s="5" t="s">
-        <v>1120</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="316" spans="1:3" ht="46.5" x14ac:dyDescent="0.35">
@@ -7042,7 +7093,7 @@
         <v>679</v>
       </c>
       <c r="C316" s="5" t="s">
-        <v>1121</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="317" spans="1:3" ht="46.5" x14ac:dyDescent="0.35">
@@ -7119,7 +7170,7 @@
         <v>690</v>
       </c>
       <c r="C323" s="5" t="s">
-        <v>1122</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="324" spans="1:3" ht="46.5" x14ac:dyDescent="0.35">
@@ -7163,7 +7214,7 @@
         <v>697</v>
       </c>
       <c r="C327" s="5" t="s">
-        <v>1123</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="328" spans="1:3" ht="46.5" x14ac:dyDescent="0.35">
@@ -7196,7 +7247,7 @@
         <v>850</v>
       </c>
       <c r="C330" s="11" t="s">
-        <v>1124</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="331" spans="1:3" ht="46.5" x14ac:dyDescent="0.35">
@@ -7207,7 +7258,7 @@
         <v>702</v>
       </c>
       <c r="C331" s="5" t="s">
-        <v>1125</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="332" spans="1:3" ht="46.5" x14ac:dyDescent="0.35">
@@ -7262,7 +7313,7 @@
         <v>851</v>
       </c>
       <c r="C336" s="11" t="s">
-        <v>1126</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="337" spans="1:3" ht="46.5" x14ac:dyDescent="0.35">
@@ -7317,7 +7368,7 @@
         <v>719</v>
       </c>
       <c r="C341" s="5" t="s">
-        <v>1127</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="342" spans="1:3" ht="46.5" x14ac:dyDescent="0.35">
@@ -7328,7 +7379,7 @@
         <v>720</v>
       </c>
       <c r="C342" s="5" t="s">
-        <v>1128</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="343" spans="1:3" ht="46.5" x14ac:dyDescent="0.35">
@@ -7361,7 +7412,7 @@
         <v>725</v>
       </c>
       <c r="C345" s="5" t="s">
-        <v>1129</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="346" spans="1:3" ht="46.5" x14ac:dyDescent="0.35">
@@ -7392,7 +7443,7 @@
         <v>728</v>
       </c>
       <c r="C348" s="5" t="s">
-        <v>1130</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="349" spans="1:3" ht="46.5" x14ac:dyDescent="0.35">
@@ -7403,7 +7454,7 @@
         <v>703</v>
       </c>
       <c r="C349" s="11" t="s">
-        <v>1131</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="350" spans="1:3" x14ac:dyDescent="0.35">
@@ -7467,7 +7518,7 @@
         <v>737</v>
       </c>
       <c r="C355" s="5" t="s">
-        <v>1132</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="356" spans="1:3" ht="46.5" x14ac:dyDescent="0.35">
@@ -7478,7 +7529,7 @@
         <v>738</v>
       </c>
       <c r="C356" s="5" t="s">
-        <v>1133</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="357" spans="1:3" ht="46.5" x14ac:dyDescent="0.35">
@@ -7500,7 +7551,7 @@
         <v>741</v>
       </c>
       <c r="C358" s="5" t="s">
-        <v>1134</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="359" spans="1:3" ht="46.5" x14ac:dyDescent="0.35">
@@ -7533,7 +7584,7 @@
         <v>746</v>
       </c>
       <c r="C361" s="5" t="s">
-        <v>1135</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="362" spans="1:3" ht="46.5" x14ac:dyDescent="0.35">
@@ -7588,7 +7639,7 @@
         <v>754</v>
       </c>
       <c r="C366" s="5" t="s">
-        <v>1136</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="367" spans="1:3" ht="46.5" x14ac:dyDescent="0.35">
@@ -7654,7 +7705,7 @@
         <v>765</v>
       </c>
       <c r="C372" s="5" t="s">
-        <v>1137</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="373" spans="1:3" ht="46.5" x14ac:dyDescent="0.35">
@@ -7727,7 +7778,7 @@
         <v>852</v>
       </c>
       <c r="C379" s="11" t="s">
-        <v>1138</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="380" spans="1:3" ht="46.5" x14ac:dyDescent="0.35">
@@ -7738,7 +7789,7 @@
         <v>771</v>
       </c>
       <c r="C380" s="5" t="s">
-        <v>1139</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="381" spans="1:3" ht="46.5" x14ac:dyDescent="0.35">
@@ -7749,7 +7800,7 @@
         <v>772</v>
       </c>
       <c r="C381" s="5" t="s">
-        <v>1140</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="382" spans="1:3" ht="46.5" x14ac:dyDescent="0.35">
@@ -7942,7 +7993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="401" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="401" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A401" s="1" t="s">
         <v>25</v>
       </c>
@@ -7950,73 +8001,73 @@
         <v>0</v>
       </c>
     </row>
-    <row r="402" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="402" spans="1:5" ht="31" x14ac:dyDescent="0.35">
       <c r="A402" s="1" t="s">
         <v>370</v>
       </c>
       <c r="B402" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="D402" s="1" t="s">
+      <c r="E402" s="1" t="s">
         <v>854</v>
       </c>
     </row>
-    <row r="403" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="403" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A403" s="1" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="404" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="404" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A404" s="1" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="405" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="405" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A405" s="1" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="406" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="406" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A406" s="1" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="407" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="407" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A407" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="408" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="408" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A408" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="409" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="409" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A409" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="410" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="410" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A410" s="1" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="411" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="411" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A411" s="1" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="412" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="412" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A412" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="413" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="413" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A413" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="414" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="414" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A414" s="1" t="s">
         <v>98</v>
       </c>
@@ -8024,7 +8075,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="415" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="415" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A415" s="1" t="s">
         <v>108</v>
       </c>
@@ -8032,7 +8083,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="416" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="416" spans="1:5" ht="31" x14ac:dyDescent="0.35">
       <c r="A416" s="1" t="s">
         <v>377</v>
       </c>
@@ -8374,7 +8425,7 @@
         <v>799</v>
       </c>
     </row>
-    <row r="449" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="449" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A449" s="1" t="s">
         <v>179</v>
       </c>
@@ -8385,7 +8436,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="450" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="450" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A450" s="1" t="s">
         <v>405</v>
       </c>
@@ -8393,10 +8444,10 @@
         <v>517</v>
       </c>
       <c r="C450" s="6" t="s">
-        <v>1141</v>
-      </c>
-    </row>
-    <row r="451" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
+        <v>1139</v>
+      </c>
+    </row>
+    <row r="451" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A451" s="1" t="s">
         <v>406</v>
       </c>
@@ -8407,7 +8458,7 @@
         <v>801</v>
       </c>
     </row>
-    <row r="452" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="452" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A452" s="1" t="s">
         <v>407</v>
       </c>
@@ -8418,7 +8469,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="453" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="453" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A453" s="1" t="s">
         <v>24</v>
       </c>
@@ -8426,7 +8477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="454" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="454" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A454" s="1" t="s">
         <v>25</v>
       </c>
@@ -8434,58 +8485,58 @@
         <v>0</v>
       </c>
     </row>
-    <row r="455" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="455" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A455" s="1" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="456" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="456" spans="1:5" ht="31" x14ac:dyDescent="0.35">
       <c r="A456" s="1" t="s">
         <v>408</v>
       </c>
       <c r="B456" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="D456" s="1" t="s">
+      <c r="E456" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="457" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="457" spans="1:5" ht="31" x14ac:dyDescent="0.35">
       <c r="A457" s="1" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="458" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="458" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A458" s="1" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="459" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="459" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A459" s="1" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="460" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="460" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A460" s="1" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="461" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="461" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A461" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="462" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="462" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A462" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="463" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="463" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A463" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="464" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="464" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A464" s="1" t="s">
         <v>413</v>
       </c>
@@ -8640,18 +8691,18 @@
         <v>814</v>
       </c>
     </row>
-    <row r="481" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="481" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A481" s="1" t="s">
         <v>429</v>
       </c>
       <c r="B481" s="6" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="C481" s="6" t="s">
         <v>815</v>
       </c>
     </row>
-    <row r="482" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="482" spans="1:5" ht="31" x14ac:dyDescent="0.35">
       <c r="A482" s="1" t="s">
         <v>430</v>
       </c>
@@ -8662,7 +8713,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="483" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="483" spans="1:5" ht="31" x14ac:dyDescent="0.35">
       <c r="A483" s="1" t="s">
         <v>431</v>
       </c>
@@ -8673,7 +8724,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="484" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="484" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A484" s="1" t="s">
         <v>26</v>
       </c>
@@ -8682,7 +8733,7 @@
       </c>
       <c r="C484" s="6"/>
     </row>
-    <row r="485" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="485" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A485" s="1" t="s">
         <v>432</v>
       </c>
@@ -8693,7 +8744,7 @@
         <v>818</v>
       </c>
     </row>
-    <row r="486" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="486" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A486" s="1" t="s">
         <v>24</v>
       </c>
@@ -8701,7 +8752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="487" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="487" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A487" s="1" t="s">
         <v>25</v>
       </c>
@@ -8709,7 +8760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="488" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="488" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A488" s="1" t="s">
         <v>433</v>
       </c>
@@ -8718,7 +8769,7 @@
       </c>
       <c r="C488" s="6"/>
     </row>
-    <row r="489" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="489" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A489" s="1" t="s">
         <v>434</v>
       </c>
@@ -8728,11 +8779,11 @@
       <c r="C489" s="6" t="s">
         <v>1026</v>
       </c>
-      <c r="D489" s="1" t="s">
-        <v>1059</v>
-      </c>
-    </row>
-    <row r="490" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E489" s="1" t="s">
+        <v>1058</v>
+      </c>
+    </row>
+    <row r="490" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A490" s="1" t="s">
         <v>435</v>
       </c>
@@ -8740,11 +8791,11 @@
         <v>0</v>
       </c>
       <c r="C490" s="6"/>
-      <c r="D490" s="1" t="s">
-        <v>1060</v>
-      </c>
-    </row>
-    <row r="491" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E490" s="1" t="s">
+        <v>1059</v>
+      </c>
+    </row>
+    <row r="491" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A491" s="1" t="s">
         <v>26</v>
       </c>
@@ -8752,11 +8803,11 @@
         <v>0</v>
       </c>
       <c r="C491" s="6"/>
-      <c r="D491" s="1" t="s">
-        <v>1061</v>
-      </c>
-    </row>
-    <row r="492" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E491" s="1" t="s">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="492" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A492" s="1" t="s">
         <v>436</v>
       </c>
@@ -8766,35 +8817,35 @@
       <c r="C492" s="6" t="s">
         <v>1026</v>
       </c>
-      <c r="D492" s="1" t="s">
-        <v>1062</v>
-      </c>
-    </row>
-    <row r="493" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E492" s="1" t="s">
+        <v>1061</v>
+      </c>
+    </row>
+    <row r="493" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A493" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B493" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D493" s="1" t="s">
-        <v>1063</v>
-      </c>
-    </row>
-    <row r="494" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E493" s="1" t="s">
+        <v>1062</v>
+      </c>
+    </row>
+    <row r="494" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A494" s="1" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="495" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="495" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A495" s="1" t="s">
         <v>437</v>
       </c>
       <c r="B495" s="5" t="s">
-        <v>1174</v>
-      </c>
-    </row>
-    <row r="496" spans="1:4" x14ac:dyDescent="0.35">
+        <v>1172</v>
+      </c>
+    </row>
+    <row r="496" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A496" s="1" t="s">
         <v>109</v>
       </c>
@@ -8807,13 +8858,13 @@
         <v>438</v>
       </c>
       <c r="B497" s="5" t="s">
-        <v>1180</v>
+        <v>1178</v>
       </c>
       <c r="C497" s="5" t="s">
-        <v>1179</v>
-      </c>
-      <c r="D497" s="1" t="s">
-        <v>1068</v>
+        <v>1177</v>
+      </c>
+      <c r="E497" s="1" t="s">
+        <v>1067</v>
       </c>
     </row>
     <row r="498" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
@@ -8821,13 +8872,13 @@
         <v>439</v>
       </c>
       <c r="B498" s="5" t="s">
-        <v>1181</v>
+        <v>1179</v>
       </c>
       <c r="C498" s="5" t="s">
-        <v>1186</v>
-      </c>
-      <c r="D498" s="1" t="s">
-        <v>1069</v>
+        <v>1184</v>
+      </c>
+      <c r="E498" s="1" t="s">
+        <v>1068</v>
       </c>
     </row>
     <row r="499" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
@@ -8835,28 +8886,28 @@
         <v>440</v>
       </c>
       <c r="B499" s="11" t="s">
-        <v>1182</v>
+        <v>1180</v>
       </c>
       <c r="C499" s="5" t="s">
-        <v>1175</v>
-      </c>
-      <c r="D499" s="1" t="s">
-        <v>1064</v>
-      </c>
-      <c r="E499" s="9"/>
+        <v>1173</v>
+      </c>
+      <c r="D499" s="9"/>
+      <c r="E499" s="1" t="s">
+        <v>1063</v>
+      </c>
     </row>
     <row r="500" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A500" s="1" t="s">
         <v>441</v>
       </c>
       <c r="B500" s="5" t="s">
-        <v>1183</v>
+        <v>1181</v>
       </c>
       <c r="C500" s="5" t="s">
-        <v>1176</v>
-      </c>
-      <c r="D500" s="1" t="s">
-        <v>1065</v>
+        <v>1174</v>
+      </c>
+      <c r="E500" s="1" t="s">
+        <v>1064</v>
       </c>
     </row>
     <row r="501" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
@@ -8864,13 +8915,13 @@
         <v>442</v>
       </c>
       <c r="B501" s="5" t="s">
-        <v>1184</v>
+        <v>1182</v>
       </c>
       <c r="C501" s="5" t="s">
-        <v>1177</v>
-      </c>
-      <c r="D501" s="1" t="s">
-        <v>1066</v>
+        <v>1175</v>
+      </c>
+      <c r="E501" s="1" t="s">
+        <v>1065</v>
       </c>
     </row>
     <row r="502" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
@@ -8878,13 +8929,13 @@
         <v>443</v>
       </c>
       <c r="B502" s="11" t="s">
-        <v>1185</v>
+        <v>1183</v>
       </c>
       <c r="C502" s="5" t="s">
-        <v>1178</v>
-      </c>
-      <c r="D502" s="1" t="s">
-        <v>1067</v>
+        <v>1176</v>
+      </c>
+      <c r="E502" s="1" t="s">
+        <v>1066</v>
       </c>
     </row>
     <row r="503" spans="1:5" x14ac:dyDescent="0.35">
@@ -8903,7 +8954,7 @@
         <v>519</v>
       </c>
       <c r="C504" s="9" t="s">
-        <v>1189</v>
+        <v>1187</v>
       </c>
     </row>
     <row r="505" spans="1:5" x14ac:dyDescent="0.35">
@@ -8968,11 +9019,11 @@
         <v>0</v>
       </c>
       <c r="C512" s="6"/>
-      <c r="D512" s="1" t="s">
-        <v>1070</v>
-      </c>
-    </row>
-    <row r="513" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+      <c r="E512" s="1" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="513" spans="1:5" ht="31" x14ac:dyDescent="0.35">
       <c r="A513" s="1" t="s">
         <v>451</v>
       </c>
@@ -8982,11 +9033,11 @@
       <c r="C513" s="6" t="s">
         <v>874</v>
       </c>
-      <c r="D513" s="1" t="s">
-        <v>1071</v>
-      </c>
-    </row>
-    <row r="514" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+      <c r="E513" s="1" t="s">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="514" spans="1:5" ht="31" x14ac:dyDescent="0.35">
       <c r="A514" s="1" t="s">
         <v>452</v>
       </c>
@@ -8996,11 +9047,11 @@
       <c r="C514" s="6" t="s">
         <v>875</v>
       </c>
-      <c r="D514" s="1" t="s">
-        <v>1072</v>
-      </c>
-    </row>
-    <row r="515" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E514" s="1" t="s">
+        <v>1071</v>
+      </c>
+    </row>
+    <row r="515" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A515" s="1" t="s">
         <v>453</v>
       </c>
@@ -9010,11 +9061,11 @@
       <c r="C515" s="6" t="s">
         <v>876</v>
       </c>
-      <c r="D515" s="1" t="s">
-        <v>1073</v>
-      </c>
-    </row>
-    <row r="516" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E515" s="1" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="516" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A516" s="1" t="s">
         <v>454</v>
       </c>
@@ -9024,11 +9075,11 @@
       <c r="C516" s="6" t="s">
         <v>877</v>
       </c>
-      <c r="D516" s="1" t="s">
-        <v>1074</v>
-      </c>
-    </row>
-    <row r="517" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E516" s="1" t="s">
+        <v>1073</v>
+      </c>
+    </row>
+    <row r="517" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A517" s="1" t="s">
         <v>455</v>
       </c>
@@ -9038,11 +9089,11 @@
       <c r="C517" s="6" t="s">
         <v>878</v>
       </c>
-      <c r="D517" s="1" t="s">
-        <v>1075</v>
-      </c>
-    </row>
-    <row r="518" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E517" s="1" t="s">
+        <v>1074</v>
+      </c>
+    </row>
+    <row r="518" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A518" s="1" t="s">
         <v>456</v>
       </c>
@@ -9052,11 +9103,11 @@
       <c r="C518" s="6" t="s">
         <v>879</v>
       </c>
-      <c r="D518" s="1" t="s">
-        <v>1076</v>
-      </c>
-    </row>
-    <row r="519" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E518" s="1" t="s">
+        <v>1075</v>
+      </c>
+    </row>
+    <row r="519" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A519" s="1" t="s">
         <v>457</v>
       </c>
@@ -9066,11 +9117,11 @@
       <c r="C519" s="6" t="s">
         <v>880</v>
       </c>
-      <c r="D519" s="1" t="s">
-        <v>1077</v>
-      </c>
-    </row>
-    <row r="520" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E519" s="1" t="s">
+        <v>1076</v>
+      </c>
+    </row>
+    <row r="520" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A520" s="1" t="s">
         <v>458</v>
       </c>
@@ -9080,11 +9131,11 @@
       <c r="C520" s="6" t="s">
         <v>881</v>
       </c>
-      <c r="D520" s="1" t="s">
-        <v>1078</v>
-      </c>
-    </row>
-    <row r="521" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E520" s="1" t="s">
+        <v>1077</v>
+      </c>
+    </row>
+    <row r="521" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A521" s="1" t="s">
         <v>459</v>
       </c>
@@ -9094,11 +9145,11 @@
       <c r="C521" s="6" t="s">
         <v>882</v>
       </c>
-      <c r="D521" s="1" t="s">
-        <v>1079</v>
-      </c>
-    </row>
-    <row r="522" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E521" s="1" t="s">
+        <v>1078</v>
+      </c>
+    </row>
+    <row r="522" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A522" s="1" t="s">
         <v>460</v>
       </c>
@@ -9108,11 +9159,11 @@
       <c r="C522" s="6" t="s">
         <v>883</v>
       </c>
-      <c r="D522" s="1" t="s">
-        <v>1080</v>
-      </c>
-    </row>
-    <row r="523" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E522" s="1" t="s">
+        <v>1079</v>
+      </c>
+    </row>
+    <row r="523" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A523" s="1" t="s">
         <v>461</v>
       </c>
@@ -9122,11 +9173,11 @@
       <c r="C523" s="6" t="s">
         <v>884</v>
       </c>
-      <c r="D523" s="1" t="s">
-        <v>1081</v>
-      </c>
-    </row>
-    <row r="524" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E523" s="1" t="s">
+        <v>1080</v>
+      </c>
+    </row>
+    <row r="524" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A524" s="1" t="s">
         <v>462</v>
       </c>
@@ -9136,11 +9187,11 @@
       <c r="C524" s="6" t="s">
         <v>885</v>
       </c>
-      <c r="D524" s="1" t="s">
-        <v>1082</v>
-      </c>
-    </row>
-    <row r="525" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E524" s="1" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="525" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A525" s="1" t="s">
         <v>26</v>
       </c>
@@ -9148,33 +9199,33 @@
         <v>0</v>
       </c>
       <c r="C525" s="6"/>
-      <c r="D525" s="1" t="s">
-        <v>1083</v>
-      </c>
-    </row>
-    <row r="526" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E525" s="1" t="s">
+        <v>1082</v>
+      </c>
+    </row>
+    <row r="526" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A526" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B526" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D526" s="1" t="s">
-        <v>1084</v>
-      </c>
-    </row>
-    <row r="527" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E526" s="1" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="527" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A527" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B527" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D527" s="1" t="s">
-        <v>1085</v>
-      </c>
-    </row>
-    <row r="528" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+      <c r="E527" s="1" t="s">
+        <v>1084</v>
+      </c>
+    </row>
+    <row r="528" spans="1:5" ht="31" x14ac:dyDescent="0.35">
       <c r="A528" s="1" t="s">
         <v>463</v>
       </c>
@@ -9185,7 +9236,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="529" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="529" spans="1:5" ht="31" x14ac:dyDescent="0.35">
       <c r="A529" s="1" t="s">
         <v>464</v>
       </c>
@@ -9195,11 +9246,11 @@
       <c r="C529" s="1" t="s">
         <v>886</v>
       </c>
-      <c r="D529" s="1" t="s">
-        <v>1086</v>
-      </c>
-    </row>
-    <row r="530" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+      <c r="E529" s="1" t="s">
+        <v>1085</v>
+      </c>
+    </row>
+    <row r="530" spans="1:5" ht="31" x14ac:dyDescent="0.35">
       <c r="A530" s="1" t="s">
         <v>465</v>
       </c>
@@ -9209,11 +9260,11 @@
       <c r="C530" s="1" t="s">
         <v>887</v>
       </c>
-      <c r="D530" s="1" t="s">
-        <v>1087</v>
-      </c>
-    </row>
-    <row r="531" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+      <c r="E530" s="1" t="s">
+        <v>1086</v>
+      </c>
+    </row>
+    <row r="531" spans="1:5" ht="31" x14ac:dyDescent="0.35">
       <c r="A531" s="1" t="s">
         <v>466</v>
       </c>
@@ -9223,11 +9274,11 @@
       <c r="C531" s="1" t="s">
         <v>888</v>
       </c>
-      <c r="D531" s="1" t="s">
-        <v>1088</v>
-      </c>
-    </row>
-    <row r="532" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E531" s="1" t="s">
+        <v>1087</v>
+      </c>
+    </row>
+    <row r="532" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A532" s="1" t="s">
         <v>25</v>
       </c>
@@ -9235,12 +9286,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="534" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="534" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A534" s="3" t="s">
         <v>467</v>
       </c>
     </row>
-    <row r="535" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="535" spans="1:5" ht="31" x14ac:dyDescent="0.35">
       <c r="A535" s="1" t="s">
         <v>468</v>
       </c>
@@ -9248,7 +9299,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="536" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="536" spans="1:5" ht="31" x14ac:dyDescent="0.35">
       <c r="A536" s="1" t="s">
         <v>469</v>
       </c>
@@ -9256,7 +9307,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="537" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="537" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A537" s="1" t="s">
         <v>470</v>
       </c>
@@ -9264,7 +9315,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="538" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="538" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A538" s="1" t="s">
         <v>471</v>
       </c>
@@ -9272,7 +9323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="539" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="539" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A539" s="1" t="s">
         <v>28</v>
       </c>
@@ -9280,7 +9331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="540" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="540" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A540" s="1" t="s">
         <v>29</v>
       </c>
@@ -9288,12 +9339,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="541" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="541" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A541" s="1" t="s">
         <v>472</v>
       </c>
     </row>
-    <row r="542" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="542" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A542" s="1" t="s">
         <v>98</v>
       </c>
@@ -9301,12 +9352,12 @@
         <v>506</v>
       </c>
     </row>
-    <row r="543" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="543" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A543" s="1" t="s">
         <v>473</v>
       </c>
     </row>
-    <row r="544" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="544" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A544" s="1" t="s">
         <v>148</v>
       </c>
@@ -9341,10 +9392,10 @@
         <v>475</v>
       </c>
       <c r="B548" s="5" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="C548" s="5" t="s">
-        <v>1142</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="549" spans="1:3" x14ac:dyDescent="0.35">
@@ -9410,7 +9461,7 @@
         <v>839</v>
       </c>
       <c r="C554" s="5" t="s">
-        <v>1143</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="555" spans="1:3" x14ac:dyDescent="0.35">
@@ -9479,7 +9530,7 @@
         <v>829</v>
       </c>
     </row>
-    <row r="561" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="561" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A561" s="1" t="s">
         <v>23</v>
       </c>
@@ -9487,10 +9538,10 @@
         <v>840</v>
       </c>
       <c r="C561" s="5" t="s">
-        <v>1144</v>
-      </c>
-    </row>
-    <row r="562" spans="1:4" x14ac:dyDescent="0.35">
+        <v>1142</v>
+      </c>
+    </row>
+    <row r="562" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A562" s="1" t="s">
         <v>482</v>
       </c>
@@ -9501,7 +9552,7 @@
         <v>830</v>
       </c>
     </row>
-    <row r="563" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="563" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A563" s="1" t="s">
         <v>32</v>
       </c>
@@ -9512,7 +9563,7 @@
         <v>831</v>
       </c>
     </row>
-    <row r="564" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="564" spans="1:5" ht="31" x14ac:dyDescent="0.35">
       <c r="A564" s="1" t="s">
         <v>33</v>
       </c>
@@ -9523,7 +9574,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="565" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="565" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A565" s="1" t="s">
         <v>43</v>
       </c>
@@ -9534,7 +9585,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="566" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="566" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A566" s="1" t="s">
         <v>483</v>
       </c>
@@ -9545,7 +9596,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="567" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="567" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A567" s="1" t="s">
         <v>24</v>
       </c>
@@ -9553,7 +9604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="568" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="568" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A568" s="1" t="s">
         <v>25</v>
       </c>
@@ -9561,15 +9612,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="569" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="569" spans="1:5" ht="31" x14ac:dyDescent="0.35">
       <c r="A569" s="1" t="s">
         <v>484</v>
       </c>
       <c r="B569" s="11" t="s">
-        <v>1156</v>
-      </c>
-    </row>
-    <row r="570" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+        <v>1154</v>
+      </c>
+    </row>
+    <row r="570" spans="1:5" ht="31" x14ac:dyDescent="0.35">
       <c r="A570" s="1" t="s">
         <v>485</v>
       </c>
@@ -9579,11 +9630,11 @@
       <c r="C570" s="6" t="s">
         <v>843</v>
       </c>
-      <c r="D570" s="1" t="s">
+      <c r="E570" s="1" t="s">
         <v>1042</v>
       </c>
     </row>
-    <row r="571" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="571" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A571" s="1" t="s">
         <v>486</v>
       </c>
@@ -9593,11 +9644,11 @@
       <c r="C571" s="6" t="s">
         <v>844</v>
       </c>
-      <c r="D571" s="1" t="s">
+      <c r="E571" s="1" t="s">
         <v>1041</v>
       </c>
     </row>
-    <row r="572" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="572" spans="1:5" ht="31" x14ac:dyDescent="0.35">
       <c r="A572" s="1" t="s">
         <v>487</v>
       </c>
@@ -9607,11 +9658,11 @@
       <c r="C572" s="6" t="s">
         <v>845</v>
       </c>
-      <c r="D572" s="1" t="s">
+      <c r="E572" s="1" t="s">
         <v>1040</v>
       </c>
     </row>
-    <row r="573" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="573" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A573" s="1" t="s">
         <v>27</v>
       </c>
@@ -9620,7 +9671,7 @@
       </c>
       <c r="C573" s="6"/>
     </row>
-    <row r="574" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="574" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A574" s="1" t="s">
         <v>26</v>
       </c>
@@ -9629,7 +9680,7 @@
       </c>
       <c r="C574" s="6"/>
     </row>
-    <row r="575" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="575" spans="1:5" ht="31" x14ac:dyDescent="0.35">
       <c r="A575" s="1" t="s">
         <v>488</v>
       </c>
@@ -9640,7 +9691,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="576" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="576" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A576" s="1" t="s">
         <v>25</v>
       </c>

</xml_diff>